<commit_message>
rebase on openurp 0.25.1
</commit_message>
<xml_diff>
--- a/audit/src/main/resources/org/openurp/std/graduation/audit/degree_apply.xlsx
+++ b/audit/src/main/resources/org/openurp/std/graduation/audit/degree_apply.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7280"/>
+    <workbookView windowWidth="19200" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>${school}学士学位申请表</t>
   </si>
@@ -131,7 +131,13 @@
 审查意见</t>
   </si>
   <si>
+    <t>${apply.auditOn1}</t>
+  </si>
+  <si>
     <t>学位评定委员会审查意见</t>
+  </si>
+  <si>
+    <t>${apply.auditOn2}</t>
   </si>
   <si>
     <t>备　注</t>
@@ -155,8 +161,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
@@ -192,6 +198,110 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -200,19 +310,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -224,118 +342,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -350,187 +356,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,6 +647,56 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,6 +706,30 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -668,80 +748,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -750,10 +756,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -762,133 +768,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1292,8 +1298,8 @@
   <sheetPr/>
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:K19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -1492,7 +1498,7 @@
     <row r="11" ht="14.15" customHeight="1" spans="1:11">
       <c r="A11" s="8"/>
       <c r="B11" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1519,7 +1525,7 @@
     </row>
     <row r="13" ht="120" customHeight="1" spans="1:11">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1535,7 +1541,7 @@
     <row r="14" ht="14.15" customHeight="1" spans="1:11">
       <c r="A14" s="8"/>
       <c r="B14" s="14" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1562,10 +1568,10 @@
     </row>
     <row r="16" ht="22.65" customHeight="1" spans="1:11">
       <c r="A16" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -1580,7 +1586,7 @@
     <row r="17" ht="22.65" customHeight="1" spans="1:11">
       <c r="A17" s="8"/>
       <c r="B17" s="16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -1595,7 +1601,7 @@
     <row r="18" ht="22.65" customHeight="1" spans="1:11">
       <c r="A18" s="8"/>
       <c r="B18" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -1609,7 +1615,7 @@
     </row>
     <row r="19" ht="97" customHeight="1" spans="1:22">
       <c r="A19" s="20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>

</xml_diff>